<commit_message>
importing and updating data in database
</commit_message>
<xml_diff>
--- a/seed_data/Confirming_matching_data.xlsx
+++ b/seed_data/Confirming_matching_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="291">
   <si>
     <t>locations</t>
   </si>
@@ -880,6 +880,18 @@
   </si>
   <si>
     <t>New Richmond, WI</t>
+  </si>
+  <si>
+    <t>Zillow</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>Biloxi</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
   </si>
 </sst>
 </file>
@@ -946,8 +958,262 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="201">
+  <cellStyleXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1156,7 +1422,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="201">
+  <cellStyles count="455">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1257,6 +1523,133 @@
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1357,6 +1750,133 @@
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1688,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="J110" sqref="J110"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="M156" sqref="M156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6148,7 +6668,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:11">
       <c r="A129" s="1" t="s">
         <v>88</v>
       </c>
@@ -6182,7 +6702,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:11">
       <c r="A130" s="1" t="s">
         <v>109</v>
       </c>
@@ -6216,7 +6736,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:11">
       <c r="A131" s="1" t="s">
         <v>110</v>
       </c>
@@ -6250,7 +6770,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:11">
       <c r="A132" s="1" t="s">
         <v>111</v>
       </c>
@@ -6284,7 +6804,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:11">
       <c r="A133" s="1" t="s">
         <v>112</v>
       </c>
@@ -6314,8 +6834,11 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:10">
+      <c r="J133" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" s="1" t="s">
         <v>113</v>
       </c>
@@ -6345,8 +6868,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:10">
+      <c r="J134" t="s">
+        <v>287</v>
+      </c>
+      <c r="K134" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" s="1" t="s">
         <v>2</v>
       </c>
@@ -6376,8 +6905,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:10">
+      <c r="J135" t="s">
+        <v>287</v>
+      </c>
+      <c r="K135" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" s="1" t="s">
         <v>114</v>
       </c>
@@ -6407,8 +6942,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:10">
+      <c r="J136" t="s">
+        <v>287</v>
+      </c>
+      <c r="K136" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="1" t="s">
         <v>115</v>
       </c>
@@ -6438,8 +6979,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:10">
+      <c r="J137" t="s">
+        <v>287</v>
+      </c>
+      <c r="K137" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="1" t="s">
         <v>116</v>
       </c>
@@ -6469,8 +7016,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:10">
+      <c r="J138" t="s">
+        <v>287</v>
+      </c>
+      <c r="K138" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="1" t="s">
         <v>117</v>
       </c>
@@ -6500,8 +7053,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:10">
+      <c r="J139" t="s">
+        <v>287</v>
+      </c>
+      <c r="K139" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" s="1" t="s">
         <v>118</v>
       </c>
@@ -6531,8 +7090,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:10">
+      <c r="J140" t="s">
+        <v>287</v>
+      </c>
+      <c r="K140" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" s="1" t="s">
         <v>119</v>
       </c>
@@ -6562,8 +7127,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:10">
+      <c r="J141" t="s">
+        <v>287</v>
+      </c>
+      <c r="K141" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" s="1" t="s">
         <v>40</v>
       </c>
@@ -6593,8 +7164,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:10">
+      <c r="J142" t="s">
+        <v>287</v>
+      </c>
+      <c r="K142" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143" s="1" t="s">
         <v>120</v>
       </c>
@@ -6624,8 +7201,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:10">
+      <c r="J143" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K143" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" s="1" t="s">
         <v>49</v>
       </c>
@@ -6655,8 +7238,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:10">
+      <c r="J144" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K144" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145" s="1" t="s">
         <v>47</v>
       </c>
@@ -6686,8 +7275,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:10">
+      <c r="J145" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K145" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146" s="1" t="s">
         <v>121</v>
       </c>
@@ -6717,8 +7312,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:10">
+      <c r="J146" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K146" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147" s="1" t="s">
         <v>87</v>
       </c>
@@ -6748,8 +7349,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:10">
+      <c r="J147" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K147" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148" s="1" t="s">
         <v>122</v>
       </c>
@@ -6779,8 +7386,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:10">
+      <c r="J148" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K148" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149" s="1" t="s">
         <v>40</v>
       </c>
@@ -6810,10 +7423,16 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:10">
+      <c r="J149" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K149" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150" s="1" t="s">
-        <v>97</v>
+        <v>289</v>
       </c>
       <c r="B150" t="s">
         <v>179</v>
@@ -6827,11 +7446,11 @@
       </c>
       <c r="F150" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G150" t="str">
         <f t="shared" si="10"/>
-        <v>MemphisMississippi</v>
+        <v>BiloxiMississippi</v>
       </c>
       <c r="H150" t="str">
         <f t="shared" si="11"/>
@@ -6839,10 +7458,16 @@
       </c>
       <c r="I150" t="b">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K150" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151" s="1" t="s">
         <v>92</v>
       </c>
@@ -6872,8 +7497,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:10">
+      <c r="J151" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K151" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152" s="1" t="s">
         <v>123</v>
       </c>
@@ -6903,8 +7534,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:10">
+      <c r="J152" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K152" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153" s="1" t="s">
         <v>88</v>
       </c>
@@ -6934,8 +7571,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:10">
+      <c r="J153" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K153" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154" s="1" t="s">
         <v>95</v>
       </c>
@@ -6965,8 +7608,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:10">
+      <c r="J154" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K154" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" s="1" t="s">
         <v>124</v>
       </c>
@@ -7000,7 +7649,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:11">
       <c r="A156" s="1" t="s">
         <v>125</v>
       </c>
@@ -7030,8 +7679,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:10">
+      <c r="J156" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K156" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157" s="1" t="s">
         <v>126</v>
       </c>
@@ -7065,7 +7720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:11">
       <c r="A158" s="1" t="s">
         <v>48</v>
       </c>
@@ -7095,8 +7750,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:10">
+      <c r="J158" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K158" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159" s="1" t="s">
         <v>127</v>
       </c>
@@ -7126,8 +7787,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:10">
+      <c r="J159" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K159" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160" s="1" t="s">
         <v>128</v>
       </c>
@@ -7157,8 +7824,14 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:10">
+      <c r="J160" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K160" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161" s="1" t="s">
         <v>64</v>
       </c>
@@ -7191,13 +7864,16 @@
       <c r="J161" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="162" spans="1:10">
+      <c r="K161" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
       <c r="A162" s="1" t="s">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="B162" t="s">
-        <v>158</v>
+        <v>290</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
@@ -7208,11 +7884,11 @@
       </c>
       <c r="F162" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G162" t="str">
         <f t="shared" si="10"/>
-        <v>ColumbiaNorth Carolina</v>
+        <v>WashingtonDistrict of Columbia</v>
       </c>
       <c r="H162" t="str">
         <f t="shared" si="11"/>
@@ -7220,10 +7896,16 @@
       </c>
       <c r="I162" t="b">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K162" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
       <c r="G163" t="str">
         <f t="shared" si="10"/>
         <v/>

</xml_diff>

<commit_message>
updated Model.py and seed.py so that the database is now connecting
</commit_message>
<xml_diff>
--- a/seed_data/Confirming_matching_data.xlsx
+++ b/seed_data/Confirming_matching_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="27340" windowHeight="16480" tabRatio="500" activeTab="1"/>
+    <workbookView minimized="1" xWindow="260" yWindow="0" windowWidth="27340" windowHeight="16480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="307">
   <si>
     <t>locations</t>
   </si>
@@ -1027,8 +1027,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="793">
+  <cellStyleXfs count="835">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1837,7 +1879,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="793">
+  <cellStyles count="835">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2234,6 +2276,27 @@
     <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2630,6 +2693,27 @@
     <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9065,10 +9149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10523,14 +10607,14 @@
         <v>146</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="I61" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D61=F61</f>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -10547,14 +10631,14 @@
         <v>146</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="I62" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D62=F62</f>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -10571,14 +10655,14 @@
         <v>147</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="I63" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D63=F63</f>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -10595,17 +10679,17 @@
         <v>147</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="I64" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -10618,18 +10702,18 @@
       <c r="E65" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F65" s="8" t="s">
-        <v>38</v>
+      <c r="F65" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="I65" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -10643,17 +10727,17 @@
         <v>148</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="I66" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>37</v>
       </c>
@@ -10667,17 +10751,17 @@
         <v>148</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="I67" t="b">
-        <f t="shared" ref="I67:I108" si="1">D67=F67</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <f t="shared" ref="I67:I77" si="1">D67=F67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -10691,17 +10775,17 @@
         <v>148</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="I68" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -10715,17 +10799,17 @@
         <v>148</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="I69" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -10739,17 +10823,17 @@
         <v>148</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="I70" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -10763,17 +10847,17 @@
         <v>129</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I71" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -10787,17 +10871,17 @@
         <v>129</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I72" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -10811,17 +10895,17 @@
         <v>129</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I73" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>44</v>
       </c>
@@ -10835,17 +10919,17 @@
         <v>149</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I74" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -10859,17 +10943,17 @@
         <v>149</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I75" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -10883,17 +10967,17 @@
         <v>149</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I76" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>46</v>
       </c>
@@ -10907,17 +10991,17 @@
         <v>149</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I77" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>47</v>
       </c>
@@ -10930,18 +11014,14 @@
       <c r="E78" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F78" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="I78" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K78" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -10954,18 +11034,8 @@
       <c r="E79" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F79" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="I79" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>49</v>
       </c>
@@ -10978,18 +11048,11 @@
       <c r="E80" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F80" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="I80" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>259</v>
       </c>
@@ -11002,18 +11065,14 @@
       <c r="E81" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F81" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G81" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I81" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K81" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -11026,18 +11085,8 @@
       <c r="E82" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F82" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I82" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -11050,18 +11099,8 @@
       <c r="E83" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="F83" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I83" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>52</v>
       </c>
@@ -11074,18 +11113,8 @@
       <c r="E84" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F84" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="I84" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>53</v>
       </c>
@@ -11098,18 +11127,8 @@
       <c r="E85" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I85" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>54</v>
       </c>
@@ -11122,18 +11141,8 @@
       <c r="E86" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F86" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I86" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -11146,18 +11155,14 @@
       <c r="E87" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F87" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="I87" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="L87" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" t="s">
         <v>56</v>
       </c>
@@ -11170,18 +11175,8 @@
       <c r="E88" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F88" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G88" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I88" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>296</v>
       </c>
@@ -11194,18 +11189,8 @@
       <c r="E89" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F89" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I89" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>58</v>
       </c>
@@ -11218,18 +11203,8 @@
       <c r="E90" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F90" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I90" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>59</v>
       </c>
@@ -11242,18 +11217,8 @@
       <c r="E91" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F91" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I91" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>60</v>
       </c>
@@ -11266,18 +11231,8 @@
       <c r="E92" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I92" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -11290,18 +11245,8 @@
       <c r="E93" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F93" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I93" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" t="s">
         <v>61</v>
       </c>
@@ -11314,18 +11259,8 @@
       <c r="E94" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F94" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I94" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>62</v>
       </c>
@@ -11338,18 +11273,8 @@
       <c r="E95" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F95" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I95" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -11362,18 +11287,8 @@
       <c r="E96" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F96" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I96" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>64</v>
       </c>
@@ -11386,18 +11301,8 @@
       <c r="E97" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I97" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -11410,18 +11315,8 @@
       <c r="E98" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F98" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I98" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>66</v>
       </c>
@@ -11434,18 +11329,8 @@
       <c r="E99" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F99" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G99" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I99" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -11458,18 +11343,8 @@
       <c r="E100" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F100" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G100" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I100" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>67</v>
       </c>
@@ -11482,18 +11357,8 @@
       <c r="E101" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F101" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G101" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I101" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>68</v>
       </c>
@@ -11506,18 +11371,8 @@
       <c r="E102" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F102" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="G102" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I102" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>69</v>
       </c>
@@ -11530,18 +11385,8 @@
       <c r="E103" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F103" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="G103" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I103" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>70</v>
       </c>
@@ -11554,18 +11399,8 @@
       <c r="E104" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F104" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="G104" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I104" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>267</v>
       </c>
@@ -11578,18 +11413,8 @@
       <c r="E105" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F105" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G105" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I105" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>268</v>
       </c>
@@ -11602,18 +11427,8 @@
       <c r="E106" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F106" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G106" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I106" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>269</v>
       </c>
@@ -11626,18 +11441,8 @@
       <c r="E107" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F107" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I107" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -11650,18 +11455,8 @@
       <c r="E108" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F108" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G108" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I108" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>64</v>
       </c>
@@ -11675,7 +11470,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>74</v>
       </c>
@@ -11689,7 +11484,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>75</v>
       </c>
@@ -11703,7 +11498,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Map limit(20) broke, so using list slicing to limit results to first 20
</commit_message>
<xml_diff>
--- a/seed_data/Confirming_matching_data.xlsx
+++ b/seed_data/Confirming_matching_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="260" yWindow="0" windowWidth="27340" windowHeight="16480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6520" yWindow="80" windowWidth="8220" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -953,7 +953,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1027,8 +1026,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="835">
+  <cellStyleXfs count="855">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1879,7 +1898,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="835">
+  <cellStyles count="855">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2297,6 +2316,16 @@
     <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2714,6 +2743,16 @@
     <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3045,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3094,11 +3133,11 @@
         <v>130</v>
       </c>
       <c r="F2" t="b">
-        <f>A2=D2</f>
+        <f t="shared" ref="F2:F33" si="0">A2=D2</f>
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f>CONCATENATE(A2,B2)</f>
+        <f t="shared" ref="G2:G33" si="1">CONCATENATE(A2,B2)</f>
         <v>BirminghamAlabama</v>
       </c>
       <c r="H2" t="str">
@@ -3131,19 +3170,19 @@
         <v>130</v>
       </c>
       <c r="F3" t="b">
-        <f>A3=D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE(A3,B3)</f>
+        <f t="shared" si="1"/>
         <v>HelenaAlabama</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="0">CONCATENATE(D3,E3)</f>
+        <f t="shared" ref="H3:H66" si="2">CONCATENATE(D3,E3)</f>
         <v>HelenaAlabama</v>
       </c>
       <c r="I3" t="b">
-        <f t="shared" ref="I3:I66" si="1">G3=H3</f>
+        <f t="shared" ref="I3:I66" si="3">G3=H3</f>
         <v>1</v>
       </c>
       <c r="J3" t="s">
@@ -3168,19 +3207,19 @@
         <v>131</v>
       </c>
       <c r="F4" t="b">
-        <f>A4=D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE(A4,B4)</f>
+        <f t="shared" si="1"/>
         <v>PeoriaArizona</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>PeoriaArizona</v>
       </c>
       <c r="I4" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J4" t="s">
@@ -3208,19 +3247,19 @@
         <v>131</v>
       </c>
       <c r="F5" t="b">
-        <f>A5=D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G5" t="str">
-        <f>CONCATENATE(A5,B5)</f>
+        <f t="shared" si="1"/>
         <v>PhoenixArizona</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>PhoenixArizona</v>
       </c>
       <c r="I5" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J5" t="s">
@@ -3245,19 +3284,19 @@
         <v>131</v>
       </c>
       <c r="F6" t="b">
-        <f>A6=D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE(A6,B6)</f>
+        <f t="shared" si="1"/>
         <v>ScottsdaleArizona</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ScottsdaleArizona</v>
       </c>
       <c r="I6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J6" t="s">
@@ -3285,19 +3324,19 @@
         <v>131</v>
       </c>
       <c r="F7" t="b">
-        <f>A7=D7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE(A7,B7)</f>
+        <f t="shared" si="1"/>
         <v>TucsonArizona</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>TusconArizona</v>
       </c>
       <c r="I7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J7" t="s">
@@ -3322,19 +3361,19 @@
         <v>132</v>
       </c>
       <c r="F8" t="b">
-        <f>A8=D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE(A8,B8)</f>
+        <f t="shared" si="1"/>
         <v>Little RockArkansas</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Little RockArkansas</v>
       </c>
       <c r="I8" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J8" t="s">
@@ -3359,19 +3398,19 @@
         <v>132</v>
       </c>
       <c r="F9" t="b">
-        <f>A9=D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE(A9,B9)</f>
+        <f t="shared" si="1"/>
         <v>North Little RockArkansas</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North Little RockArkansas</v>
       </c>
       <c r="I9" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J9" t="s">
@@ -3399,19 +3438,19 @@
         <v>133</v>
       </c>
       <c r="F10" t="b">
-        <f>A10=D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE(A10,B10)</f>
+        <f t="shared" si="1"/>
         <v>Los AngelesCalifornia</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Los AngelesCalifornia</v>
       </c>
       <c r="I10" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J10" t="s">
@@ -3436,19 +3475,19 @@
         <v>133</v>
       </c>
       <c r="F11" t="b">
-        <f>A11=D11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G11" t="str">
-        <f>CONCATENATE(A11,B11)</f>
+        <f t="shared" si="1"/>
         <v>NewarkCalifornia</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>NewarkCalifornia</v>
       </c>
       <c r="I11" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -3476,19 +3515,19 @@
         <v>133</v>
       </c>
       <c r="F12" t="b">
-        <f>A12=D12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G12" t="str">
-        <f>CONCATENATE(A12,B12)</f>
+        <f t="shared" si="1"/>
         <v>OaklandCalifornia</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>OaklandCalifornia</v>
       </c>
       <c r="I12" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J12" t="s">
@@ -3513,19 +3552,19 @@
         <v>133</v>
       </c>
       <c r="F13" t="b">
-        <f>A13=D13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G13" t="str">
-        <f>CONCATENATE(A13,B13)</f>
+        <f t="shared" si="1"/>
         <v>RichmondCalifornia</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>RichmondCalifornia</v>
       </c>
       <c r="I13" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J13" t="s">
@@ -3553,19 +3592,19 @@
         <v>133</v>
       </c>
       <c r="F14" t="b">
-        <f>A14=D14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G14" t="str">
-        <f>CONCATENATE(A14,B14)</f>
+        <f t="shared" si="1"/>
         <v>RiversideCalifornia</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>RiversideCalifornia</v>
       </c>
       <c r="I14" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J14" t="s">
@@ -3590,19 +3629,19 @@
         <v>133</v>
       </c>
       <c r="F15" t="b">
-        <f>A15=D15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G15" t="str">
-        <f>CONCATENATE(A15,B15)</f>
+        <f t="shared" si="1"/>
         <v>SacramentoCalifornia</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>SacramentoCalifornia</v>
       </c>
       <c r="I15" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J15" t="s">
@@ -3627,19 +3666,19 @@
         <v>133</v>
       </c>
       <c r="F16" t="b">
-        <f>A16=D16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G16" t="str">
-        <f>CONCATENATE(A16,B16)</f>
+        <f t="shared" si="1"/>
         <v>San FranciscoCalifornia</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>San FranciscoCalifornia</v>
       </c>
       <c r="I16" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J16" t="s">
@@ -3664,19 +3703,19 @@
         <v>133</v>
       </c>
       <c r="F17" t="b">
-        <f>A17=D17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G17" t="str">
-        <f>CONCATENATE(A17,B17)</f>
+        <f t="shared" si="1"/>
         <v>San JoseCalifornia</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>San JoseCalifornia</v>
       </c>
       <c r="I17" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J17" t="s">
@@ -3701,19 +3740,19 @@
         <v>133</v>
       </c>
       <c r="F18" t="b">
-        <f>A18=D18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G18" t="str">
-        <f>CONCATENATE(A18,B18)</f>
+        <f t="shared" si="1"/>
         <v>South San FranciscoCalifornia</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>South San FranciscoCalifornia</v>
       </c>
       <c r="I18" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J18" t="s">
@@ -3741,19 +3780,19 @@
         <v>134</v>
       </c>
       <c r="F19" t="b">
-        <f>A19=D19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G19" t="str">
-        <f>CONCATENATE(A19,B19)</f>
+        <f t="shared" si="1"/>
         <v>AuroraColorado</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>AuroraColorado</v>
       </c>
       <c r="I19" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J19" t="s">
@@ -3781,19 +3820,19 @@
         <v>134</v>
       </c>
       <c r="F20" t="b">
-        <f>A20=D20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G20" t="str">
-        <f>CONCATENATE(A20,B20)</f>
+        <f t="shared" si="1"/>
         <v>BoulderColorado</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BoulderColorado</v>
       </c>
       <c r="I20" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J20" t="s">
@@ -3818,19 +3857,19 @@
         <v>134</v>
       </c>
       <c r="F21" t="b">
-        <f>A21=D21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G21" t="str">
-        <f>CONCATENATE(A21,B21)</f>
+        <f t="shared" si="1"/>
         <v>DenverColorado</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>DenverColorado</v>
       </c>
       <c r="I21" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J21" t="s">
@@ -3855,19 +3894,19 @@
         <v>134</v>
       </c>
       <c r="F22" t="b">
-        <f>A22=D22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" t="str">
-        <f>CONCATENATE(A22,B22)</f>
+        <f t="shared" si="1"/>
         <v>LafayetteColorado</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>LayfayetteColorado</v>
       </c>
       <c r="I22" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J22" t="s">
@@ -3892,19 +3931,19 @@
         <v>134</v>
       </c>
       <c r="F23" s="4" t="b">
-        <f>A23=D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="4" t="str">
-        <f>CONCATENATE(A23,B23)</f>
+        <f t="shared" si="1"/>
         <v>Colorado SpringsColorado</v>
       </c>
       <c r="H23" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ColumbiaColorado</v>
       </c>
       <c r="I23" s="4" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
@@ -3932,19 +3971,19 @@
         <v>135</v>
       </c>
       <c r="F24" t="b">
-        <f>A24=D24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G24" t="str">
-        <f>CONCATENATE(A24,B24)</f>
+        <f t="shared" si="1"/>
         <v>BridgeportConnecitcut</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BridgeportConnecitcut</v>
       </c>
       <c r="I24" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J24" t="s">
@@ -3969,19 +4008,19 @@
         <v>135</v>
       </c>
       <c r="F25" t="b">
-        <f>A25=D25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G25" t="str">
-        <f>CONCATENATE(A25,B25)</f>
+        <f t="shared" si="1"/>
         <v>GreenwichConnecitcut</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>GreenwichConnecitcut</v>
       </c>
       <c r="I25" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J25" t="s">
@@ -4009,19 +4048,19 @@
         <v>135</v>
       </c>
       <c r="F26" t="b">
-        <f>A26=D26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G26" t="str">
-        <f>CONCATENATE(A26,B26)</f>
+        <f t="shared" si="1"/>
         <v>HartfordConnecitcut</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>HartfordConnecitcut</v>
       </c>
       <c r="I26" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J26" t="s">
@@ -4049,19 +4088,19 @@
         <v>135</v>
       </c>
       <c r="F27" t="b">
-        <f>A27=D27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G27" t="str">
-        <f>CONCATENATE(A27,B27)</f>
+        <f t="shared" si="1"/>
         <v>New HavenConnecitcut</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>New HavenConnecitcut</v>
       </c>
       <c r="I27" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J27" t="s">
@@ -4086,19 +4125,19 @@
         <v>136</v>
       </c>
       <c r="F28" t="b">
-        <f>A28=D28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G28" t="str">
-        <f>CONCATENATE(A28,B28)</f>
+        <f t="shared" si="1"/>
         <v>DoverDelaware</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>DoverDelaware</v>
       </c>
       <c r="I28" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J28" t="s">
@@ -4123,19 +4162,19 @@
         <v>136</v>
       </c>
       <c r="F29" t="b">
-        <f>A29=D29</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G29" t="str">
-        <f>CONCATENATE(A29,B29)</f>
+        <f t="shared" si="1"/>
         <v>NewarkDelaware</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>NewarkDelaware</v>
       </c>
       <c r="I29" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J29" t="s">
@@ -4160,19 +4199,19 @@
         <v>136</v>
       </c>
       <c r="F30" t="b">
-        <f>A30=D30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G30" t="str">
-        <f>CONCATENATE(A30,B30)</f>
+        <f t="shared" si="1"/>
         <v>WilmingtonDelaware</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>WilmingtonDelaware</v>
       </c>
       <c r="I30" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J30" t="s">
@@ -4197,19 +4236,19 @@
         <v>137</v>
       </c>
       <c r="F31" t="b">
-        <f>A31=D31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G31" t="str">
-        <f>CONCATENATE(A31,B31)</f>
+        <f t="shared" si="1"/>
         <v>JacksonvilleFlorida</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>JacksonvilleFlorida</v>
       </c>
       <c r="I31" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J31" t="s">
@@ -4234,19 +4273,19 @@
         <v>137</v>
       </c>
       <c r="F32" t="b">
-        <f>A32=D32</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G32" t="str">
-        <f>CONCATENATE(A32,B32)</f>
+        <f t="shared" si="1"/>
         <v>Jacksonville BeachFlorida</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Jacksonville BeachFlorida</v>
       </c>
       <c r="I32" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J32" t="s">
@@ -4271,19 +4310,19 @@
         <v>137</v>
       </c>
       <c r="F33" t="b">
-        <f>A33=D33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G33" t="str">
-        <f>CONCATENATE(A33,B33)</f>
+        <f t="shared" si="1"/>
         <v>MiamiFlorida</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>MiamiFlorida</v>
       </c>
       <c r="I33" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J33" t="s">
@@ -4308,19 +4347,19 @@
         <v>137</v>
       </c>
       <c r="F34" t="b">
-        <f>A34=D34</f>
+        <f t="shared" ref="F34:F65" si="4">A34=D34</f>
         <v>1</v>
       </c>
       <c r="G34" t="str">
-        <f>CONCATENATE(A34,B34)</f>
+        <f t="shared" ref="G34:G65" si="5">CONCATENATE(A34,B34)</f>
         <v>Miami BeachFlorida</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Miami BeachFlorida</v>
       </c>
       <c r="I34" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J34" t="s">
@@ -4348,19 +4387,19 @@
         <v>137</v>
       </c>
       <c r="F35" t="b">
-        <f>A35=D35</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G35" t="str">
-        <f>CONCATENATE(A35,B35)</f>
+        <f t="shared" si="5"/>
         <v>North MiamiFlorida</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North MiamiFlorida</v>
       </c>
       <c r="I35" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J35" t="s">
@@ -4388,19 +4427,19 @@
         <v>137</v>
       </c>
       <c r="F36" t="b">
-        <f>A36=D36</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G36" t="str">
-        <f>CONCATENATE(A36,B36)</f>
+        <f t="shared" si="5"/>
         <v>North Miami BeachFlorida</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North Miami BeachFlorida</v>
       </c>
       <c r="I36" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J36" t="s">
@@ -4428,19 +4467,19 @@
         <v>137</v>
       </c>
       <c r="F37" t="b">
-        <f>A37=D37</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G37" t="str">
-        <f>CONCATENATE(A37,B37)</f>
+        <f t="shared" si="5"/>
         <v>OrlandoFlorida</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>OrlandoFlorida</v>
       </c>
       <c r="I37" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J37" t="s">
@@ -4465,19 +4504,19 @@
         <v>137</v>
       </c>
       <c r="F38" t="b">
-        <f>A38=D38</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G38" t="str">
-        <f>CONCATENATE(A38,B38)</f>
+        <f t="shared" si="5"/>
         <v>South MiamiFlorida</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>South MiamiFlorida</v>
       </c>
       <c r="I38" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J38" t="s">
@@ -4502,19 +4541,19 @@
         <v>137</v>
       </c>
       <c r="F39" t="b">
-        <f>A39=D39</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G39" t="str">
-        <f>CONCATENATE(A39,B39)</f>
+        <f t="shared" si="5"/>
         <v>TampaFlorida</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>TampaFlorida</v>
       </c>
       <c r="I39" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J39" t="s">
@@ -4539,19 +4578,19 @@
         <v>138</v>
       </c>
       <c r="F40" t="b">
-        <f>A40=D40</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G40" t="str">
-        <f>CONCATENATE(A40,B40)</f>
+        <f t="shared" si="5"/>
         <v>AtlantaGeorgia</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>AtlantaGeorgia</v>
       </c>
       <c r="I40" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J40" t="s">
@@ -4576,19 +4615,19 @@
         <v>138</v>
       </c>
       <c r="F41" t="b">
-        <f>A41=D41</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G41" t="str">
-        <f>CONCATENATE(A41,B41)</f>
+        <f t="shared" si="5"/>
         <v>FayettevilleGeorgia</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FayettevilleGeorgia</v>
       </c>
       <c r="I41" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J41" t="s">
@@ -4613,19 +4652,19 @@
         <v>138</v>
       </c>
       <c r="F42" t="b">
-        <f>A42=D42</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G42" t="str">
-        <f>CONCATENATE(A42,B42)</f>
+        <f t="shared" si="5"/>
         <v>JacksonGeorgia</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>JacksonGeorgia</v>
       </c>
       <c r="I42" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J42" t="s">
@@ -4650,19 +4689,19 @@
         <v>138</v>
       </c>
       <c r="F43" t="b">
-        <f>A43=D43</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G43" t="str">
-        <f>CONCATENATE(A43,B43)</f>
+        <f t="shared" si="5"/>
         <v>North AtlantaGeorgia</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North AtlantaGeorgia</v>
       </c>
       <c r="I43" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J43" t="s">
@@ -4687,19 +4726,19 @@
         <v>139</v>
       </c>
       <c r="F44" t="b">
-        <f>A44=D44</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G44" t="str">
-        <f>CONCATENATE(A44,B44)</f>
+        <f t="shared" si="5"/>
         <v>East HonoluluHawaii</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>East HonoluluHawaii</v>
       </c>
       <c r="I44" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J44" t="s">
@@ -4727,19 +4766,19 @@
         <v>139</v>
       </c>
       <c r="F45" t="b">
-        <f>A45=D45</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G45" t="str">
-        <f>CONCATENATE(A45,B45)</f>
+        <f t="shared" si="5"/>
         <v>HonoluluHawaii</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>HonoluluHawaii</v>
       </c>
       <c r="I45" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J45" t="s">
@@ -4764,19 +4803,19 @@
         <v>140</v>
       </c>
       <c r="F46" t="b">
-        <f>A46=D46</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G46" t="str">
-        <f>CONCATENATE(A46,B46)</f>
+        <f t="shared" si="5"/>
         <v>BoiseIdaho</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BoiseIdaho</v>
       </c>
       <c r="I46" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J46" t="s">
@@ -4801,19 +4840,19 @@
         <v>141</v>
       </c>
       <c r="F47" t="b">
-        <f>A47=D47</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G47" t="str">
-        <f>CONCATENATE(A47,B47)</f>
+        <f t="shared" si="5"/>
         <v>AuroraIllinois</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>AuroraIllinois</v>
       </c>
       <c r="I47" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J47" t="s">
@@ -4841,19 +4880,19 @@
         <v>141</v>
       </c>
       <c r="F48" t="b">
-        <f>A48=D48</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G48" t="str">
-        <f>CONCATENATE(A48,B48)</f>
+        <f t="shared" si="5"/>
         <v>ChicagoIllinois</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ChicagoIllinois</v>
       </c>
       <c r="I48" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J48" t="s">
@@ -4878,19 +4917,19 @@
         <v>141</v>
       </c>
       <c r="F49" t="b">
-        <f>A49=D49</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G49" t="str">
-        <f>CONCATENATE(A49,B49)</f>
+        <f t="shared" si="5"/>
         <v>Chicago HeightsIllinois</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Chicago HeightsIllinois</v>
       </c>
       <c r="I49" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J49" t="s">
@@ -4915,19 +4954,19 @@
         <v>141</v>
       </c>
       <c r="F50" t="b">
-        <f>A50=D50</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G50" t="str">
-        <f>CONCATENATE(A50,B50)</f>
+        <f t="shared" si="5"/>
         <v>FrankfortIllinois</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FrankfortIllinois</v>
       </c>
       <c r="I50" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J50" t="s">
@@ -4955,19 +4994,19 @@
         <v>141</v>
       </c>
       <c r="F51" t="b">
-        <f>A51=D51</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G51" t="str">
-        <f>CONCATENATE(A51,B51)</f>
+        <f t="shared" si="5"/>
         <v>LansingIllinois</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>LansingIllinois</v>
       </c>
       <c r="I51" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J51" t="s">
@@ -4992,19 +5031,19 @@
         <v>141</v>
       </c>
       <c r="F52" t="b">
-        <f>A52=D52</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G52" t="str">
-        <f>CONCATENATE(A52,B52)</f>
+        <f t="shared" si="5"/>
         <v>MontgomeryIllinois</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>MontgomeryIllinois</v>
       </c>
       <c r="I52" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J52" t="s">
@@ -5029,19 +5068,19 @@
         <v>141</v>
       </c>
       <c r="F53" t="b">
-        <f>A53=D53</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G53" t="str">
-        <f>CONCATENATE(A53,B53)</f>
+        <f t="shared" si="5"/>
         <v>North AuroraIllinois</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North AuroraIllinois</v>
       </c>
       <c r="I53" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J53" t="s">
@@ -5066,19 +5105,19 @@
         <v>141</v>
       </c>
       <c r="F54" t="b">
-        <f>A54=D54</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G54" t="str">
-        <f>CONCATENATE(A54,B54)</f>
+        <f t="shared" si="5"/>
         <v>North ChicagoIllinois</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>North ChicagoIllinois</v>
       </c>
       <c r="I54" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J54" t="s">
@@ -5103,19 +5142,19 @@
         <v>141</v>
       </c>
       <c r="F55" t="b">
-        <f>A55=D55</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G55" t="str">
-        <f>CONCATENATE(A55,B55)</f>
+        <f t="shared" si="5"/>
         <v>West ChicagoIllinois</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>West ChicagoIllinois</v>
       </c>
       <c r="I55" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J55" t="s">
@@ -5140,19 +5179,19 @@
         <v>142</v>
       </c>
       <c r="F56" t="b">
-        <f>A56=D56</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G56" t="str">
-        <f>CONCATENATE(A56,B56)</f>
+        <f t="shared" si="5"/>
         <v>IndianapolisIndiana</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>IndianapolisIndiana</v>
       </c>
       <c r="I56" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J56" t="s">
@@ -5177,19 +5216,19 @@
         <v>143</v>
       </c>
       <c r="F57" t="b">
-        <f>A57=D57</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G57" t="str">
-        <f>CONCATENATE(A57,B57)</f>
+        <f t="shared" si="5"/>
         <v>Des MoinesIowa</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Des MoinesIowa</v>
       </c>
       <c r="I57" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J57" t="s">
@@ -5214,19 +5253,19 @@
         <v>143</v>
       </c>
       <c r="F58" t="b">
-        <f>A58=D58</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G58" t="str">
-        <f>CONCATENATE(A58,B58)</f>
+        <f t="shared" si="5"/>
         <v>West Des MoinesIowa</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>West Des MoinesIowa</v>
       </c>
       <c r="I58" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J58" t="s">
@@ -5254,19 +5293,19 @@
         <v>144</v>
       </c>
       <c r="F59" t="b">
-        <f>A59=D59</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G59" t="str">
-        <f>CONCATENATE(A59,B59)</f>
+        <f t="shared" si="5"/>
         <v>Kansas CityKansas</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Kansas CityKansas</v>
       </c>
       <c r="I59" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J59" t="s">
@@ -5294,19 +5333,19 @@
         <v>145</v>
       </c>
       <c r="F60" t="b">
-        <f>A60=D60</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G60" t="str">
-        <f>CONCATENATE(A60,B60)</f>
+        <f t="shared" si="5"/>
         <v>LouisvilleKentucky</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>LouisvilleKentucky</v>
       </c>
       <c r="I60" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J60" t="s">
@@ -5331,19 +5370,19 @@
         <v>146</v>
       </c>
       <c r="F61" t="b">
-        <f>A61=D61</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G61" t="str">
-        <f>CONCATENATE(A61,B61)</f>
+        <f t="shared" si="5"/>
         <v>JeffersonLouisiana</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>JeffersonLouisiana</v>
       </c>
       <c r="I61" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J61" t="s">
@@ -5368,19 +5407,19 @@
         <v>146</v>
       </c>
       <c r="F62" t="b">
-        <f>A62=D62</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G62" t="str">
-        <f>CONCATENATE(A62,B62)</f>
+        <f t="shared" si="5"/>
         <v>New OrleansLouisiana</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>New OrleansLouisiana</v>
       </c>
       <c r="I62" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J62" t="s">
@@ -5405,19 +5444,19 @@
         <v>147</v>
       </c>
       <c r="F63" t="b">
-        <f>A63=D63</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G63" t="str">
-        <f>CONCATENATE(A63,B63)</f>
+        <f t="shared" si="5"/>
         <v>AnnapolisMaryland</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>AnnapolisMaryland</v>
       </c>
       <c r="I63" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J63" t="s">
@@ -5442,19 +5481,19 @@
         <v>147</v>
       </c>
       <c r="F64" t="b">
-        <f>A64=D64</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G64" t="str">
-        <f>CONCATENATE(A64,B64)</f>
+        <f t="shared" si="5"/>
         <v>BaltimoreMaryland</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BaltimoreMaryland</v>
       </c>
       <c r="I64" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J64" t="s">
@@ -5479,19 +5518,19 @@
         <v>147</v>
       </c>
       <c r="F65" t="b">
-        <f>A65=D65</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G65" t="str">
-        <f>CONCATENATE(A65,B65)</f>
+        <f t="shared" si="5"/>
         <v>ColumbiaMaryland</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ColumbiaMaryland</v>
       </c>
       <c r="I65" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J65" t="s">
@@ -5519,19 +5558,19 @@
         <v>148</v>
       </c>
       <c r="F66" t="b">
-        <f>A66=D66</f>
+        <f t="shared" ref="F66:F97" si="6">A66=D66</f>
         <v>1</v>
       </c>
       <c r="G66" t="str">
-        <f>CONCATENATE(A66,B66)</f>
+        <f t="shared" ref="G66:G97" si="7">CONCATENATE(A66,B66)</f>
         <v>BostonMassachusetts</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BostonMassachusetts</v>
       </c>
       <c r="I66" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J66" t="s">
@@ -5556,19 +5595,19 @@
         <v>148</v>
       </c>
       <c r="F67" t="b">
-        <f>A67=D67</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G67" t="str">
-        <f>CONCATENATE(A67,B67)</f>
+        <f t="shared" si="7"/>
         <v>BurlingtonMassachusetts</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H130" si="2">CONCATENATE(D67,E67)</f>
+        <f t="shared" ref="H67:H130" si="8">CONCATENATE(D67,E67)</f>
         <v>BurlingtonMassachusetts</v>
       </c>
       <c r="I67" t="b">
-        <f t="shared" ref="I67:I130" si="3">G67=H67</f>
+        <f t="shared" ref="I67:I130" si="9">G67=H67</f>
         <v>1</v>
       </c>
       <c r="J67" t="s">
@@ -5596,19 +5635,19 @@
         <v>148</v>
       </c>
       <c r="F68" t="b">
-        <f>A68=D68</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G68" t="str">
-        <f>CONCATENATE(A68,B68)</f>
+        <f t="shared" si="7"/>
         <v>ConcordMassachusetts</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ConcordMassachusetts</v>
       </c>
       <c r="I68" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J68" t="s">
@@ -5633,19 +5672,19 @@
         <v>148</v>
       </c>
       <c r="F69" t="b">
-        <f>A69=D69</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G69" t="str">
-        <f>CONCATENATE(A69,B69)</f>
+        <f t="shared" si="7"/>
         <v>ManchesterMassachusetts</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ManchesterMassachusetts</v>
       </c>
       <c r="I69" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J69" t="s">
@@ -5670,19 +5709,19 @@
         <v>148</v>
       </c>
       <c r="F70" t="b">
-        <f>A70=D70</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G70" t="str">
-        <f>CONCATENATE(A70,B70)</f>
+        <f t="shared" si="7"/>
         <v>SalemMassachusetts</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SalemMassachusetts</v>
       </c>
       <c r="I70" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J70" t="s">
@@ -5707,19 +5746,19 @@
         <v>129</v>
       </c>
       <c r="F71" t="b">
-        <f>A71=D71</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G71" t="str">
-        <f>CONCATENATE(A71,B71)</f>
+        <f t="shared" si="7"/>
         <v>DetroitMichigan</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>DetroitMichigan</v>
       </c>
       <c r="I71" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J71" t="s">
@@ -5744,19 +5783,19 @@
         <v>129</v>
       </c>
       <c r="F72" t="b">
-        <f>A72=D72</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G72" t="str">
-        <f>CONCATENATE(A72,B72)</f>
+        <f t="shared" si="7"/>
         <v>BirminghamMichigan</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>BirminghamMichigan</v>
       </c>
       <c r="I72" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J72" t="s">
@@ -5784,19 +5823,19 @@
         <v>129</v>
       </c>
       <c r="F73" t="b">
-        <f>A73=D73</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G73" t="str">
-        <f>CONCATENATE(A73,B73)</f>
+        <f t="shared" si="7"/>
         <v>TrentonMichigan</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>TrentonMichigan</v>
       </c>
       <c r="I73" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J73" t="s">
@@ -5821,19 +5860,19 @@
         <v>149</v>
       </c>
       <c r="F74" t="b">
-        <f>A74=D74</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G74" t="str">
-        <f>CONCATENATE(A74,B74)</f>
+        <f t="shared" si="7"/>
         <v>BloomingtonMinnesota</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>BloomingtonMinnesota</v>
       </c>
       <c r="I74" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J74" t="s">
@@ -5861,19 +5900,19 @@
         <v>149</v>
       </c>
       <c r="F75" t="b">
-        <f>A75=D75</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G75" t="str">
-        <f>CONCATENATE(A75,B75)</f>
+        <f t="shared" si="7"/>
         <v>Columbia HeightsMinnesota</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Columbia HeightsMinnesota</v>
       </c>
       <c r="I75" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J75" t="s">
@@ -5901,19 +5940,19 @@
         <v>149</v>
       </c>
       <c r="F76" t="b">
-        <f>A76=D76</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G76" t="str">
-        <f>CONCATENATE(A76,B76)</f>
+        <f t="shared" si="7"/>
         <v>MinneapolisMinnesota</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>MinneapolisMinnesota</v>
       </c>
       <c r="I76" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J76" t="s">
@@ -5938,19 +5977,19 @@
         <v>149</v>
       </c>
       <c r="F77" t="b">
-        <f>A77=D77</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G77" t="str">
-        <f>CONCATENATE(A77,B77)</f>
+        <f t="shared" si="7"/>
         <v>South St PaulMinnesota</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>South St PaulMinnesota</v>
       </c>
       <c r="I77" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J77" t="s">
@@ -5978,19 +6017,19 @@
         <v>149</v>
       </c>
       <c r="F78" t="b">
-        <f>A78=D78</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G78" t="str">
-        <f>CONCATENATE(A78,B78)</f>
+        <f t="shared" si="7"/>
         <v>St PaulMinnesota</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>St PaulMinnesota</v>
       </c>
       <c r="I78" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J78" t="s">
@@ -6018,19 +6057,19 @@
         <v>149</v>
       </c>
       <c r="F79" t="b">
-        <f>A79=D79</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G79" t="str">
-        <f>CONCATENATE(A79,B79)</f>
+        <f t="shared" si="7"/>
         <v>West St PaulMinnesota</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>West St PaulMinnesota</v>
       </c>
       <c r="I79" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J79" t="s">
@@ -6055,19 +6094,19 @@
         <v>150</v>
       </c>
       <c r="F80" t="b">
-        <f>A80=D80</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G80" t="str">
-        <f>CONCATENATE(A80,B80)</f>
+        <f t="shared" si="7"/>
         <v>Kansas CityMissouri</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Kansas CityMissouri</v>
       </c>
       <c r="I80" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J80" t="s">
@@ -6092,19 +6131,19 @@
         <v>150</v>
       </c>
       <c r="F81" t="b">
-        <f>A81=D81</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G81" t="str">
-        <f>CONCATENATE(A81,B81)</f>
+        <f t="shared" si="7"/>
         <v>ManchesterMissouri</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ManchesterMissouri</v>
       </c>
       <c r="I81" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J81" t="s">
@@ -6129,19 +6168,19 @@
         <v>150</v>
       </c>
       <c r="F82" t="b">
-        <f>A82=D82</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G82" t="str">
-        <f>CONCATENATE(A82,B82)</f>
+        <f t="shared" si="7"/>
         <v>North Kansas CityMissouri</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>North Kansas CityMissouri</v>
       </c>
       <c r="I82" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J82" t="s">
@@ -6169,19 +6208,19 @@
         <v>151</v>
       </c>
       <c r="F83" t="b">
-        <f>A83=D83</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G83" t="str">
-        <f>CONCATENATE(A83,B83)</f>
+        <f t="shared" si="7"/>
         <v>OmahaNebraska</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>OmahaNebraska</v>
       </c>
       <c r="I83" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J83" t="s">
@@ -6206,19 +6245,19 @@
         <v>152</v>
       </c>
       <c r="F84" t="b">
-        <f>A84=D84</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G84" t="str">
-        <f>CONCATENATE(A84,B84)</f>
+        <f t="shared" si="7"/>
         <v>Las VegasNevada</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Las VegasNevada</v>
       </c>
       <c r="I84" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J84" t="s">
@@ -6243,19 +6282,19 @@
         <v>152</v>
       </c>
       <c r="F85" t="b">
-        <f>A85=D85</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G85" t="str">
-        <f>CONCATENATE(A85,B85)</f>
+        <f t="shared" si="7"/>
         <v>North Las VegasNevada</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>North Las VegasNevada</v>
       </c>
       <c r="I85" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J85" t="s">
@@ -6283,19 +6322,19 @@
         <v>153</v>
       </c>
       <c r="F86" t="b">
-        <f>A86=D86</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G86" t="str">
-        <f>CONCATENATE(A86,B86)</f>
+        <f t="shared" si="7"/>
         <v>ManchesterNew Hampshire</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ManchesterNew Hampshire</v>
       </c>
       <c r="I86" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J86" t="s">
@@ -6320,19 +6359,19 @@
         <v>153</v>
       </c>
       <c r="F87" t="b">
-        <f>A87=D87</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G87" t="str">
-        <f>CONCATENATE(A87,B87)</f>
+        <f t="shared" si="7"/>
         <v>SalemNew Hampshire</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SalemNew Hampshire</v>
       </c>
       <c r="I87" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J87" t="s">
@@ -6360,19 +6399,19 @@
         <v>154</v>
       </c>
       <c r="F88" t="b">
-        <f>A88=D88</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G88" t="str">
-        <f>CONCATENATE(A88,B88)</f>
+        <f t="shared" si="7"/>
         <v>BurlingtonNew Jersey</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>BurlingtonNew Jersey</v>
       </c>
       <c r="I88" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J88" t="s">
@@ -6397,19 +6436,19 @@
         <v>154</v>
       </c>
       <c r="F89" t="b">
-        <f>A89=D89</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G89" t="str">
-        <f>CONCATENATE(A89,B89)</f>
+        <f t="shared" si="7"/>
         <v>TrentonNew Jersey</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>TrentonNew Jersey</v>
       </c>
       <c r="I89" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J89" t="s">
@@ -6434,19 +6473,19 @@
         <v>155</v>
       </c>
       <c r="F90" t="b">
-        <f>A90=D90</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G90" t="str">
-        <f>CONCATENATE(A90,B90)</f>
+        <f t="shared" si="7"/>
         <v>Santa FeNew Mexico</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Santa FeNew Mexico</v>
       </c>
       <c r="I90" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J90" t="s">
@@ -6468,19 +6507,19 @@
         <v>156</v>
       </c>
       <c r="F91" t="b">
-        <f>A91=D91</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G91" t="str">
-        <f>CONCATENATE(A91,B91)</f>
+        <f t="shared" si="7"/>
         <v>AlbanyNew York</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>AlbanyNew York</v>
       </c>
       <c r="I91" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J91" t="s">
@@ -6502,19 +6541,19 @@
         <v>157</v>
       </c>
       <c r="F92" t="b">
-        <f>A92=D92</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G92" t="str">
-        <f>CONCATENATE(A92,B92)</f>
+        <f t="shared" si="7"/>
         <v>CharlotteeNorth Carolina</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>CharlotteeNorth Carolina</v>
       </c>
       <c r="I92" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J92" t="s">
@@ -6539,19 +6578,19 @@
         <v>157</v>
       </c>
       <c r="F93" t="b">
-        <f>A93=D93</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G93" t="str">
-        <f>CONCATENATE(A93,B93)</f>
+        <f t="shared" si="7"/>
         <v>ConcordNorth Carolina</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ConcordNorth Carolina</v>
       </c>
       <c r="I93" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J93" t="s">
@@ -6579,19 +6618,19 @@
         <v>157</v>
       </c>
       <c r="F94" t="b">
-        <f>A94=D94</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G94" t="str">
-        <f>CONCATENATE(A94,B94)</f>
+        <f t="shared" si="7"/>
         <v>DenverNorth Carolina</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>DenverNorth Carolina</v>
       </c>
       <c r="I94" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J94" t="s">
@@ -6616,19 +6655,19 @@
         <v>157</v>
       </c>
       <c r="F95" t="b">
-        <f>A95=D95</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G95" t="str">
-        <f>CONCATENATE(A95,B95)</f>
+        <f t="shared" si="7"/>
         <v>DurhamNorth Carolina</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>DurhamNorth Carolina</v>
       </c>
       <c r="I95" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J95" t="s">
@@ -6653,19 +6692,19 @@
         <v>157</v>
       </c>
       <c r="F96" t="b">
-        <f>A96=D96</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G96" t="str">
-        <f>CONCATENATE(A96,B96)</f>
+        <f t="shared" si="7"/>
         <v>HarrisburgNorth Carolina</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>HarrisburgNorth Carolina</v>
       </c>
       <c r="I96" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J96" t="s">
@@ -6693,19 +6732,19 @@
         <v>157</v>
       </c>
       <c r="F97" t="b">
-        <f>A97=D97</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G97" t="str">
-        <f>CONCATENATE(A97,B97)</f>
+        <f t="shared" si="7"/>
         <v>RaleighNorth Carolina</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>RaleighNorth Carolina</v>
       </c>
       <c r="I97" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J97" t="s">
@@ -6730,19 +6769,19 @@
         <v>158</v>
       </c>
       <c r="F98" t="b">
-        <f>A98=D98</f>
+        <f t="shared" ref="F98:F129" si="10">A98=D98</f>
         <v>1</v>
       </c>
       <c r="G98" t="str">
-        <f>CONCATENATE(A98,B98)</f>
+        <f t="shared" ref="G98:G129" si="11">CONCATENATE(A98,B98)</f>
         <v>ColumbusOhio</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ColumbusOhio</v>
       </c>
       <c r="I98" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J98" t="s">
@@ -6770,19 +6809,19 @@
         <v>158</v>
       </c>
       <c r="F99" t="b">
-        <f>A99=D99</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G99" t="str">
-        <f>CONCATENATE(A99,B99)</f>
+        <f t="shared" si="11"/>
         <v>NewarkOhio</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NewarkOhio</v>
       </c>
       <c r="I99" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J99" t="s">
@@ -6807,19 +6846,19 @@
         <v>159</v>
       </c>
       <c r="F100" t="b">
-        <f>A100=D100</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G100" t="str">
-        <f>CONCATENATE(A100,B100)</f>
+        <f t="shared" si="11"/>
         <v>Oklahoma CityOklahoma</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Oklahoma CityOklahoma</v>
       </c>
       <c r="I100" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J100" t="s">
@@ -6847,19 +6886,19 @@
         <v>160</v>
       </c>
       <c r="F101" t="b">
-        <f>A101=D101</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G101" t="str">
-        <f>CONCATENATE(A101,B101)</f>
+        <f t="shared" si="11"/>
         <v>AlbanyOregon</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>AlbanyOregon</v>
       </c>
       <c r="I101" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J101" t="s">
@@ -6884,19 +6923,19 @@
         <v>160</v>
       </c>
       <c r="F102" t="b">
-        <f>A102=D102</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G102" t="str">
-        <f>CONCATENATE(A102,B102)</f>
+        <f t="shared" si="11"/>
         <v>PortlandOregon</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>PortlandOregon</v>
       </c>
       <c r="I102" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J102" t="s">
@@ -6921,19 +6960,19 @@
         <v>160</v>
       </c>
       <c r="F103" t="b">
-        <f>A103=D103</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G103" t="str">
-        <f>CONCATENATE(A103,B103)</f>
+        <f t="shared" si="11"/>
         <v>SalemOregon</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SalemOregon</v>
       </c>
       <c r="I103" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J103" t="s">
@@ -6958,19 +6997,19 @@
         <v>160</v>
       </c>
       <c r="F104" t="b">
-        <f>A104=D104</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G104" t="str">
-        <f>CONCATENATE(A104,B104)</f>
+        <f t="shared" si="11"/>
         <v>SpringfieldOregon</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SpringfieldOregon</v>
       </c>
       <c r="I104" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J104" t="s">
@@ -6998,19 +7037,19 @@
         <v>161</v>
       </c>
       <c r="F105" t="b">
-        <f>A105=D105</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G105" t="str">
-        <f>CONCATENATE(A105,B105)</f>
+        <f t="shared" si="11"/>
         <v>HarrisburgPennsylvania</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>HarrisburgPennsylvania</v>
       </c>
       <c r="I105" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J105" t="s">
@@ -7035,19 +7074,19 @@
         <v>161</v>
       </c>
       <c r="F106" t="b">
-        <f>A106=D106</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G106" t="str">
-        <f>CONCATENATE(A106,B106)</f>
+        <f t="shared" si="11"/>
         <v>PhilidelphiaPennsylvania</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>PhilidelphiaPennsylvania</v>
       </c>
       <c r="I106" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J106" t="s">
@@ -7072,19 +7111,19 @@
         <v>162</v>
       </c>
       <c r="F107" t="b">
-        <f>A107=D107</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G107" t="str">
-        <f>CONCATENATE(A107,B107)</f>
+        <f t="shared" si="11"/>
         <v>East GreenwichRhode Island</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>East GreenwichRhode Island</v>
       </c>
       <c r="I107" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J107" t="s">
@@ -7109,19 +7148,19 @@
         <v>162</v>
       </c>
       <c r="F108" t="b">
-        <f>A108=D108</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G108" t="str">
-        <f>CONCATENATE(A108,B108)</f>
+        <f t="shared" si="11"/>
         <v>East ProvidenceRhode Island</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>East ProvidenceRhode Island</v>
       </c>
       <c r="I108" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J108" t="s">
@@ -7146,19 +7185,19 @@
         <v>162</v>
       </c>
       <c r="F109" t="b">
-        <f>A109=D109</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G109" t="str">
-        <f>CONCATENATE(A109,B109)</f>
+        <f t="shared" si="11"/>
         <v>LincolnRhode Island</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>LincolnRhode Island</v>
       </c>
       <c r="I109" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J109" t="s">
@@ -7183,19 +7222,19 @@
         <v>162</v>
       </c>
       <c r="F110" t="b">
-        <f>A110=D110</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G110" t="str">
-        <f>CONCATENATE(A110,B110)</f>
+        <f t="shared" si="11"/>
         <v>North ProvidenceRhode Island</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>North ProvidenceRhode Island</v>
       </c>
       <c r="I110" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J110" t="s">
@@ -7223,19 +7262,19 @@
         <v>162</v>
       </c>
       <c r="F111" t="b">
-        <f>A111=D111</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G111" t="str">
-        <f>CONCATENATE(A111,B111)</f>
+        <f t="shared" si="11"/>
         <v>ProvidenceRhode Island</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ProvidenceRhode Island</v>
       </c>
       <c r="I111" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J111" t="s">
@@ -7260,19 +7299,19 @@
         <v>163</v>
       </c>
       <c r="F112" t="b">
-        <f>A112=D112</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G112" t="str">
-        <f>CONCATENATE(A112,B112)</f>
+        <f t="shared" si="11"/>
         <v>CharlestonSouth Carolina</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>CharlestonSouth Carolina</v>
       </c>
       <c r="I112" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J112" t="s">
@@ -7297,19 +7336,19 @@
         <v>163</v>
       </c>
       <c r="F113" t="b">
-        <f>A113=D113</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G113" t="str">
-        <f>CONCATENATE(A113,B113)</f>
+        <f t="shared" si="11"/>
         <v>North CharlestonSouth Carolina</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>North CharlestonSouth Carolina</v>
       </c>
       <c r="I113" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J113" t="s">
@@ -7334,19 +7373,19 @@
         <v>164</v>
       </c>
       <c r="F114" t="b">
-        <f>A114=D114</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G114" t="str">
-        <f>CONCATENATE(A114,B114)</f>
+        <f t="shared" si="11"/>
         <v>MemphisTennessee</v>
       </c>
       <c r="H114" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>MemphisTennessee</v>
       </c>
       <c r="I114" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J114" t="s">
@@ -7371,19 +7410,19 @@
         <v>164</v>
       </c>
       <c r="F115" t="b">
-        <f>A115=D115</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G115" t="str">
-        <f>CONCATENATE(A115,B115)</f>
+        <f t="shared" si="11"/>
         <v>NashvilleTennessee</v>
       </c>
       <c r="H115" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NashvilleTennessee</v>
       </c>
       <c r="I115" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J115" t="s">
@@ -7408,19 +7447,19 @@
         <v>165</v>
       </c>
       <c r="F116" t="b">
-        <f>A116=D116</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G116" t="str">
-        <f>CONCATENATE(A116,B116)</f>
+        <f t="shared" si="11"/>
         <v>AustinTexas</v>
       </c>
       <c r="H116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>AustinTexas</v>
       </c>
       <c r="I116" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J116" t="s">
@@ -7445,19 +7484,19 @@
         <v>165</v>
       </c>
       <c r="F117" t="b">
-        <f>A117=D117</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G117" t="str">
-        <f>CONCATENATE(A117,B117)</f>
+        <f t="shared" si="11"/>
         <v>DallasTexas</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>DallasTexas</v>
       </c>
       <c r="I117" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J117" t="s">
@@ -7482,19 +7521,19 @@
         <v>165</v>
       </c>
       <c r="F118" t="b">
-        <f>A118=D118</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G118" t="str">
-        <f>CONCATENATE(A118,B118)</f>
+        <f t="shared" si="11"/>
         <v>Fort WorthTexas</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Fort WorthTexas</v>
       </c>
       <c r="I118" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J118" t="s">
@@ -7519,19 +7558,19 @@
         <v>165</v>
       </c>
       <c r="F119" t="b">
-        <f>A119=D119</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G119" t="str">
-        <f>CONCATENATE(A119,B119)</f>
+        <f t="shared" si="11"/>
         <v>HoustonTexas</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>HoustonTexas</v>
       </c>
       <c r="I119" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J119" t="s">
@@ -7556,19 +7595,19 @@
         <v>165</v>
       </c>
       <c r="F120" t="b">
-        <f>A120=D120</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G120" t="str">
-        <f>CONCATENATE(A120,B120)</f>
+        <f t="shared" si="11"/>
         <v>RichmondTexas</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>RichmondTexas</v>
       </c>
       <c r="I120" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J120" t="s">
@@ -7593,19 +7632,19 @@
         <v>166</v>
       </c>
       <c r="F121" t="b">
-        <f>A121=D121</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G121" t="str">
-        <f>CONCATENATE(A121,B121)</f>
+        <f t="shared" si="11"/>
         <v>ProvoUtah</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>ProvoUtah</v>
       </c>
       <c r="I121" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J121" t="s">
@@ -7630,19 +7669,19 @@
         <v>166</v>
       </c>
       <c r="F122" t="b">
-        <f>A122=D122</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G122" t="str">
-        <f>CONCATENATE(A122,B122)</f>
+        <f t="shared" si="11"/>
         <v>Salt Lake CityUtah</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Salt Lake CityUtah</v>
       </c>
       <c r="I122" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J122" t="s">
@@ -7667,19 +7706,19 @@
         <v>167</v>
       </c>
       <c r="F123" t="b">
-        <f>A123=D123</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G123" t="str">
-        <f>CONCATENATE(A123,B123)</f>
+        <f t="shared" si="11"/>
         <v>BurlingtonVermont</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>BurlingtonVermont</v>
       </c>
       <c r="I123" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J123" t="s">
@@ -7704,19 +7743,19 @@
         <v>167</v>
       </c>
       <c r="F124" t="b">
-        <f>A124=D124</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G124" t="str">
-        <f>CONCATENATE(A124,B124)</f>
+        <f t="shared" si="11"/>
         <v>South BurlingtonVermont</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>South BurlingtonVermont</v>
       </c>
       <c r="I124" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J124" t="s">
@@ -7744,19 +7783,19 @@
         <v>168</v>
       </c>
       <c r="F125" t="b">
-        <f>A125=D125</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G125" t="str">
-        <f>CONCATENATE(A125,B125)</f>
+        <f t="shared" si="11"/>
         <v>RichmondVirginia</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>RichmondVirginia</v>
       </c>
       <c r="I125" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J125" t="s">
@@ -7781,19 +7820,19 @@
         <v>168</v>
       </c>
       <c r="F126" t="b">
-        <f>A126=D126</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G126" t="str">
-        <f>CONCATENATE(A126,B126)</f>
+        <f t="shared" si="11"/>
         <v>Virginia BeachVirginia</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Virginia BeachVirginia</v>
       </c>
       <c r="I126" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J126" t="s">
@@ -7818,19 +7857,19 @@
         <v>169</v>
       </c>
       <c r="F127" t="b">
-        <f>A127=D127</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G127" t="str">
-        <f>CONCATENATE(A127,B127)</f>
+        <f t="shared" si="11"/>
         <v>OlympiaWashington</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>OlympiaWashington</v>
       </c>
       <c r="I127" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J127" t="s">
@@ -7855,19 +7894,19 @@
         <v>169</v>
       </c>
       <c r="F128" t="b">
-        <f>A128=D128</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G128" t="str">
-        <f>CONCATENATE(A128,B128)</f>
+        <f t="shared" si="11"/>
         <v>Seattle, WA metro areaWashington</v>
       </c>
       <c r="H128" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SeattleWashington</v>
       </c>
       <c r="I128" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J128" t="s">
@@ -7892,19 +7931,19 @@
         <v>170</v>
       </c>
       <c r="F129" t="b">
-        <f>A129=D129</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G129" t="str">
-        <f>CONCATENATE(A129,B129)</f>
+        <f t="shared" si="11"/>
         <v>SpringfieldWest Virginia</v>
       </c>
       <c r="H129" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>SpringfieldWest Virginia</v>
       </c>
       <c r="I129" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J129" t="s">
@@ -7929,19 +7968,19 @@
         <v>171</v>
       </c>
       <c r="F130" t="b">
-        <f>A130=D130</f>
+        <f t="shared" ref="F130:F162" si="12">A130=D130</f>
         <v>1</v>
       </c>
       <c r="G130" t="str">
-        <f>CONCATENATE(A130,B130)</f>
+        <f t="shared" ref="G130:G162" si="13">CONCATENATE(A130,B130)</f>
         <v>MadisonWisconsin</v>
       </c>
       <c r="H130" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>MadisonWisconsin</v>
       </c>
       <c r="I130" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J130" t="s">
@@ -7966,19 +8005,19 @@
         <v>171</v>
       </c>
       <c r="F131" t="b">
-        <f>A131=D131</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G131" t="str">
-        <f>CONCATENATE(A131,B131)</f>
+        <f t="shared" si="13"/>
         <v>MilwaukeeWisconsin</v>
       </c>
       <c r="H131" t="str">
-        <f t="shared" ref="H131:H163" si="4">CONCATENATE(D131,E131)</f>
+        <f t="shared" ref="H131:H163" si="14">CONCATENATE(D131,E131)</f>
         <v>MilwaukeeWisconsin</v>
       </c>
       <c r="I131" t="b">
-        <f t="shared" ref="I131:I163" si="5">G131=H131</f>
+        <f t="shared" ref="I131:I163" si="15">G131=H131</f>
         <v>1</v>
       </c>
       <c r="J131" t="s">
@@ -8003,19 +8042,19 @@
         <v>171</v>
       </c>
       <c r="F132" t="b">
-        <f>A132=D132</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G132" t="str">
-        <f>CONCATENATE(A132,B132)</f>
+        <f t="shared" si="13"/>
         <v>New RichmondWisconsin</v>
       </c>
       <c r="H132" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>New RichmondWisconsin</v>
       </c>
       <c r="I132" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J132" t="s">
@@ -8040,19 +8079,19 @@
         <v>172</v>
       </c>
       <c r="F133" t="b">
-        <f>A133=D133</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G133" t="str">
-        <f>CONCATENATE(A133,B133)</f>
+        <f t="shared" si="13"/>
         <v>JuneauAlaska</v>
       </c>
       <c r="H133" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>JuneauAlaska</v>
       </c>
       <c r="I133" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J133" t="s">
@@ -8074,19 +8113,19 @@
         <v>172</v>
       </c>
       <c r="F134" t="b">
-        <f>A134=D134</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G134" t="str">
-        <f>CONCATENATE(A134,B134)</f>
+        <f t="shared" si="13"/>
         <v>AnchorageAlaska</v>
       </c>
       <c r="H134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>AnchorageAlaska</v>
       </c>
       <c r="I134" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J134" t="s">
@@ -8111,19 +8150,19 @@
         <v>173</v>
       </c>
       <c r="F135" t="b">
-        <f>A135=D135</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G135" t="str">
-        <f>CONCATENATE(A135,B135)</f>
+        <f t="shared" si="13"/>
         <v>HelenaMontana</v>
       </c>
       <c r="H135" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>HelenaMontana</v>
       </c>
       <c r="I135" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J135" t="s">
@@ -8148,19 +8187,19 @@
         <v>173</v>
       </c>
       <c r="F136" t="b">
-        <f>A136=D136</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G136" t="str">
-        <f>CONCATENATE(A136,B136)</f>
+        <f t="shared" si="13"/>
         <v>BillingsMontana</v>
       </c>
       <c r="H136" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>BillingsMontana</v>
       </c>
       <c r="I136" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J136" t="s">
@@ -8185,19 +8224,19 @@
         <v>174</v>
       </c>
       <c r="F137" t="b">
-        <f>A137=D137</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G137" t="str">
-        <f>CONCATENATE(A137,B137)</f>
+        <f t="shared" si="13"/>
         <v>FargoNorth Dakota</v>
       </c>
       <c r="H137" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>FargoNorth Dakota</v>
       </c>
       <c r="I137" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J137" t="s">
@@ -8222,19 +8261,19 @@
         <v>174</v>
       </c>
       <c r="F138" t="b">
-        <f>A138=D138</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G138" t="str">
-        <f>CONCATENATE(A138,B138)</f>
+        <f t="shared" si="13"/>
         <v>BismarckNorth Dakota</v>
       </c>
       <c r="H138" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>BismarckNorth Dakota</v>
       </c>
       <c r="I138" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J138" t="s">
@@ -8259,19 +8298,19 @@
         <v>175</v>
       </c>
       <c r="F139" t="b">
-        <f>A139=D139</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G139" t="str">
-        <f>CONCATENATE(A139,B139)</f>
+        <f t="shared" si="13"/>
         <v>Rapid CitySouth Dakota</v>
       </c>
       <c r="H139" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>Rapid CitySouth Dakota</v>
       </c>
       <c r="I139" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J139" t="s">
@@ -8296,19 +8335,19 @@
         <v>175</v>
       </c>
       <c r="F140" t="b">
-        <f>A140=D140</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G140" t="str">
-        <f>CONCATENATE(A140,B140)</f>
+        <f t="shared" si="13"/>
         <v>Sioux FallsSouth Dakota</v>
       </c>
       <c r="H140" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>Sioux FallsSouth Dakota</v>
       </c>
       <c r="I140" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J140" t="s">
@@ -8333,19 +8372,19 @@
         <v>176</v>
       </c>
       <c r="F141" t="b">
-        <f>A141=D141</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G141" t="str">
-        <f>CONCATENATE(A141,B141)</f>
+        <f t="shared" si="13"/>
         <v>CheyenneWyoming</v>
       </c>
       <c r="H141" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>CheyenneWyoming</v>
       </c>
       <c r="I141" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J141" t="s">
@@ -8370,19 +8409,19 @@
         <v>176</v>
       </c>
       <c r="F142" t="b">
-        <f>A142=D142</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G142" t="str">
-        <f>CONCATENATE(A142,B142)</f>
+        <f t="shared" si="13"/>
         <v>JacksonWyoming</v>
       </c>
       <c r="H142" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>JacksonWyoming</v>
       </c>
       <c r="I142" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J142" t="s">
@@ -8407,19 +8446,19 @@
         <v>137</v>
       </c>
       <c r="F143" t="b">
-        <f>A143=D143</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G143" t="str">
-        <f>CONCATENATE(A143,B143)</f>
+        <f t="shared" si="13"/>
         <v>TallahasseeFlorida</v>
       </c>
       <c r="H143" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>TallahasseeFlorida</v>
       </c>
       <c r="I143" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J143" s="1" t="s">
@@ -8444,19 +8483,19 @@
         <v>130</v>
       </c>
       <c r="F144" t="b">
-        <f>A144=D144</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G144" t="str">
-        <f>CONCATENATE(A144,B144)</f>
+        <f t="shared" si="13"/>
         <v>MontgomeryAlabama</v>
       </c>
       <c r="H144" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>MontgomeryAlabama</v>
       </c>
       <c r="I144" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J144" s="1" t="s">
@@ -8481,19 +8520,19 @@
         <v>145</v>
       </c>
       <c r="F145" t="b">
-        <f>A145=D145</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G145" t="str">
-        <f>CONCATENATE(A145,B145)</f>
+        <f t="shared" si="13"/>
         <v>FrankfortKentucky</v>
       </c>
       <c r="H145" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>FrankfortKentucky</v>
       </c>
       <c r="I145" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J145" s="1" t="s">
@@ -8518,19 +8557,19 @@
         <v>177</v>
       </c>
       <c r="F146" t="b">
-        <f>A146=D146</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G146" t="str">
-        <f>CONCATENATE(A146,B146)</f>
+        <f t="shared" si="13"/>
         <v>AugustaMaine</v>
       </c>
       <c r="H146" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>AugustaMaine</v>
       </c>
       <c r="I146" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J146" s="1" t="s">
@@ -8555,19 +8594,19 @@
         <v>177</v>
       </c>
       <c r="F147" t="b">
-        <f>A147=D147</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G147" t="str">
-        <f>CONCATENATE(A147,B147)</f>
+        <f t="shared" si="13"/>
         <v>PortlandMaine</v>
       </c>
       <c r="H147" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>PortlandMaine</v>
       </c>
       <c r="I147" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J147" s="1" t="s">
@@ -8592,19 +8631,19 @@
         <v>177</v>
       </c>
       <c r="F148" t="b">
-        <f>A148=D148</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G148" t="str">
-        <f>CONCATENATE(A148,B148)</f>
+        <f t="shared" si="13"/>
         <v>South PortlandMaine</v>
       </c>
       <c r="H148" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>South PortlandMaine</v>
       </c>
       <c r="I148" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J148" s="1" t="s">
@@ -8629,19 +8668,19 @@
         <v>178</v>
       </c>
       <c r="F149" t="b">
-        <f>A149=D149</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G149" t="str">
-        <f>CONCATENATE(A149,B149)</f>
+        <f t="shared" si="13"/>
         <v>JacksonMississippi</v>
       </c>
       <c r="H149" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>JacksonMississippi</v>
       </c>
       <c r="I149" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J149" s="1" t="s">
@@ -8666,19 +8705,19 @@
         <v>178</v>
       </c>
       <c r="F150" t="b">
-        <f>A150=D150</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G150" t="str">
-        <f>CONCATENATE(A150,B150)</f>
+        <f t="shared" si="13"/>
         <v>BiloxiMississippi</v>
       </c>
       <c r="H150" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>MemphisMississippi</v>
       </c>
       <c r="I150" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J150" s="1" t="s">
@@ -8703,19 +8742,19 @@
         <v>151</v>
       </c>
       <c r="F151" t="b">
-        <f>A151=D151</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G151" t="str">
-        <f>CONCATENATE(A151,B151)</f>
+        <f t="shared" si="13"/>
         <v>LincolnNebraska</v>
       </c>
       <c r="H151" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>LincolnNebraska</v>
       </c>
       <c r="I151" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J151" s="1" t="s">
@@ -8740,19 +8779,19 @@
         <v>155</v>
       </c>
       <c r="F152" t="b">
-        <f>A152=D152</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G152" t="str">
-        <f>CONCATENATE(A152,B152)</f>
+        <f t="shared" si="13"/>
         <v>AlbuquerqueNew Mexico</v>
       </c>
       <c r="H152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>AlbuquerqueNew Mexico</v>
       </c>
       <c r="I152" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J152" s="1" t="s">
@@ -8777,19 +8816,19 @@
         <v>141</v>
       </c>
       <c r="F153" t="b">
-        <f>A153=D153</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G153" t="str">
-        <f>CONCATENATE(A153,B153)</f>
+        <f t="shared" si="13"/>
         <v>SpringfieldIllinois</v>
       </c>
       <c r="H153" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>SpringfieldIllinois</v>
       </c>
       <c r="I153" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J153" s="1" t="s">
@@ -8814,19 +8853,19 @@
         <v>170</v>
       </c>
       <c r="F154" t="b">
-        <f>A154=D154</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G154" t="str">
-        <f>CONCATENATE(A154,B154)</f>
+        <f t="shared" si="13"/>
         <v>CharlestonWest Virginia</v>
       </c>
       <c r="H154" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>CharlestonWest Virginia</v>
       </c>
       <c r="I154" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J154" s="1" t="s">
@@ -8851,19 +8890,19 @@
         <v>161</v>
       </c>
       <c r="F155" t="b">
-        <f>A155=D155</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G155" t="str">
-        <f>CONCATENATE(A155,B155)</f>
+        <f t="shared" si="13"/>
         <v>PittsburghPennsylvania</v>
       </c>
       <c r="H155" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>PittsburghPennsylvania</v>
       </c>
       <c r="I155" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J155" t="s">
@@ -8885,19 +8924,19 @@
         <v>144</v>
       </c>
       <c r="F156" t="b">
-        <f>A156=D156</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G156" t="str">
-        <f>CONCATENATE(A156,B156)</f>
+        <f t="shared" si="13"/>
         <v>TopekaKansas</v>
       </c>
       <c r="H156" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>TopekaKansas</v>
       </c>
       <c r="I156" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J156" s="1" t="s">
@@ -8922,19 +8961,19 @@
         <v>146</v>
       </c>
       <c r="F157" t="b">
-        <f>A157=D157</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G157" t="str">
-        <f>CONCATENATE(A157,B157)</f>
+        <f t="shared" si="13"/>
         <v>Baton RougeLouisiana</v>
       </c>
       <c r="H157" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>Baton RougeLouisiana</v>
       </c>
       <c r="I157" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J157" t="s">
@@ -8956,19 +8995,19 @@
         <v>129</v>
       </c>
       <c r="F158" t="b">
-        <f>A158=D158</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G158" t="str">
-        <f>CONCATENATE(A158,B158)</f>
+        <f t="shared" si="13"/>
         <v>LansingMichigan</v>
       </c>
       <c r="H158" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>LansingMichigan</v>
       </c>
       <c r="I158" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J158" s="1" t="s">
@@ -8993,19 +9032,19 @@
         <v>150</v>
       </c>
       <c r="F159" t="b">
-        <f>A159=D159</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G159" t="str">
-        <f>CONCATENATE(A159,B159)</f>
+        <f t="shared" si="13"/>
         <v>Jefferson CityMissouri</v>
       </c>
       <c r="H159" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>Jefferson CityMissouri</v>
       </c>
       <c r="I159" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J159" s="1" t="s">
@@ -9030,19 +9069,19 @@
         <v>152</v>
       </c>
       <c r="F160" t="b">
-        <f>A160=D160</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G160" t="str">
-        <f>CONCATENATE(A160,B160)</f>
+        <f t="shared" si="13"/>
         <v>Carson CityNevada</v>
       </c>
       <c r="H160" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>Carson CityNevada</v>
       </c>
       <c r="I160" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J160" s="1" t="s">
@@ -9067,19 +9106,19 @@
         <v>153</v>
       </c>
       <c r="F161" t="b">
-        <f>A161=D161</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G161" t="str">
-        <f>CONCATENATE(A161,B161)</f>
+        <f t="shared" si="13"/>
         <v>ConcordNew Hampshire</v>
       </c>
       <c r="H161" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>ConcordNew Hampshire</v>
       </c>
       <c r="I161" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J161" t="s">
@@ -9104,19 +9143,19 @@
         <v>287</v>
       </c>
       <c r="F162" t="b">
-        <f>A162=D162</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G162" t="str">
-        <f>CONCATENATE(A162,B162)</f>
+        <f t="shared" si="13"/>
         <v>WashingtonDistrict of Columbia</v>
       </c>
       <c r="H162" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>WashingtonDistrict of Columbia</v>
       </c>
       <c r="I162" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J162" s="1" t="s">
@@ -9128,11 +9167,11 @@
     </row>
     <row r="163" spans="1:11">
       <c r="H163" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I163" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -9151,8 +9190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="L104" sqref="L104"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>